<commit_message>
Integrate DB with UI and calculate user profile
</commit_message>
<xml_diff>
--- a/assets/data/material_database.xlsx
+++ b/assets/data/material_database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sonja Heinemann\Desktop\MDZ\BGF (neu)\dokuworks\App_Cardafit\Datenbasis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="254" documentId="13_ncr:1_{CFAE8855-9BD5-486C-A6AB-92984DF1B149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAB1C7A6-3BAF-4D57-B250-5CC4381268BA}"/>
+  <xr:revisionPtr revIDLastSave="303" documentId="13_ncr:1_{CFAE8855-9BD5-486C-A6AB-92984DF1B149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D519FE58-3373-44B5-A5E8-94B60058F681}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{8F0DE851-F842-4BBC-95B8-EB3CBEE83BF9}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="331">
   <si>
     <t>Steps</t>
   </si>
@@ -202,42 +202,24 @@
     <t>Setz dich auf die vordere Kante des Bürostuhls</t>
   </si>
   <si>
-    <t>08:48 - 08:52</t>
-  </si>
-  <si>
     <t>Stelle die Beine auseinader gebreitet auf</t>
   </si>
   <si>
-    <t>08:52 - 08:54</t>
-  </si>
-  <si>
     <t>Lasse deinen Oberkörper sanft nach vorne und unten fallen</t>
   </si>
   <si>
-    <t>08:54 - 09:02</t>
-  </si>
-  <si>
     <t>Lasse deine Arme und deinen Kopf locker, entspannt Richtung Boden baummeln</t>
   </si>
   <si>
-    <t>09:02 - 09:15</t>
-  </si>
-  <si>
     <t>Nach ca. 10 Sekunden Oberkörper wieder aufrichten</t>
   </si>
   <si>
-    <t>09:15 - 09:22</t>
-  </si>
-  <si>
     <t>Step 6</t>
   </si>
   <si>
     <t>Lasse deinen Oberkörper erneut sanft nach vorne und unten fallen</t>
   </si>
   <si>
-    <t>09:22 - 09:44</t>
-  </si>
-  <si>
     <t>Step 7</t>
   </si>
   <si>
@@ -253,42 +235,24 @@
     <t>Schulterbreiter Stand, Zehenspitzen nach vorne gerichtet</t>
   </si>
   <si>
-    <t>00:46 - 00:51</t>
-  </si>
-  <si>
     <t>Arme nach oben (optional, mit oder ohne Gewicht)</t>
   </si>
   <si>
-    <t>00:51 - 00:56</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gesäß nach unten Richtung Boden absenken </t>
   </si>
   <si>
-    <t>00:56 - 01:00</t>
-  </si>
-  <si>
     <t>Wichtig:Knien müssen hinter den Füßen bleiben &amp; Rücken gerade</t>
   </si>
   <si>
     <t>Nach oben aufrichten mit geradem Rücken</t>
   </si>
   <si>
-    <t>01:00 - 01:02</t>
-  </si>
-  <si>
     <t>Beide Arme gerade nach oben strecken</t>
   </si>
   <si>
-    <t>01:02 - 01:05</t>
-  </si>
-  <si>
     <t>Stärkung der Bauchmuskulatur</t>
   </si>
   <si>
-    <t>02:00 - 03:00</t>
-  </si>
-  <si>
     <t>Füße auf den Boden stellen im rechten Winkel</t>
   </si>
   <si>
@@ -310,33 +274,18 @@
     <t>Stelle dich hinter deinen Bürostuhl</t>
   </si>
   <si>
-    <t xml:space="preserve">03:03 - 03:14 </t>
-  </si>
-  <si>
     <t>Arme oben auf die Armlehne ablegen</t>
   </si>
   <si>
-    <t>03:14 - 03:15</t>
-  </si>
-  <si>
     <t>Rücken in die waagerechte Position bringen</t>
   </si>
   <si>
-    <t>03:15 - 03:18</t>
-  </si>
-  <si>
     <t>Rechtes Knie 90 Grad winkelig nach oben bringen</t>
   </si>
   <si>
-    <t>03:18 - 03:24</t>
-  </si>
-  <si>
     <t>Mit Fußsohle an die Decke zu drücken (auf und ab Bewegungen; ca. 20-30 Mal)</t>
   </si>
   <si>
-    <t>03:24 - 04:04</t>
-  </si>
-  <si>
     <t>Seite Wechseln: Linkes Knie 90 Grad winkelig nach oben bringen</t>
   </si>
   <si>
@@ -349,30 +298,18 @@
     <t>Hände auf die Tischfläche stützen</t>
   </si>
   <si>
-    <t>04:14 - 04:16</t>
-  </si>
-  <si>
     <t>Beide Füße leicht nach vorne gerichtet ausstrecken</t>
   </si>
   <si>
-    <t>04:16 - 04:17</t>
-  </si>
-  <si>
     <t>https://www.dtb.de/fileadmin/_processed_/a/5/csm_BeActivePoster_S_Dips_02_f1d234bafd.jpg</t>
   </si>
   <si>
     <t>Ellebogen gerade nach hinten geführt beugen</t>
   </si>
   <si>
-    <t>04:17 - 04:24</t>
-  </si>
-  <si>
     <t>Ellebogen auf und ab bewegen (ein paar Widerholungen)</t>
   </si>
   <si>
-    <t>04:24 - 05:11</t>
-  </si>
-  <si>
     <t>Stuhlbeuge</t>
   </si>
   <si>
@@ -481,27 +418,15 @@
     <t xml:space="preserve">Kinn zur Brust </t>
   </si>
   <si>
-    <t>06:37 - 06:42 Min.</t>
-  </si>
-  <si>
     <t>Mit geraden Rücken sitzen</t>
   </si>
   <si>
-    <t>06:42 - 06:46 Min.</t>
-  </si>
-  <si>
     <t>Kinn auf die Brust absenken</t>
   </si>
   <si>
-    <t>06:46 - 06:50 Min.</t>
-  </si>
-  <si>
     <t>Optional: Druck sanft mit Händen an den Hinterkopf erhöhen</t>
   </si>
   <si>
-    <t>06:50 - 07:37</t>
-  </si>
-  <si>
     <t>Position für ca. 20-30 Sekunden halten (bewusst Atmen)</t>
   </si>
   <si>
@@ -511,37 +436,19 @@
     <t>Steh von deinem Bürostuhl auf</t>
   </si>
   <si>
-    <t>07:41: 07:44</t>
-  </si>
-  <si>
     <t>Lege deinen rechten Arm hinter den Rücken</t>
   </si>
   <si>
-    <t>07:44 : 07:47</t>
-  </si>
-  <si>
     <t xml:space="preserve">Greife mit der anderen Hand deinen Ellebogen </t>
   </si>
   <si>
-    <t>07:47 : 07:50</t>
-  </si>
-  <si>
     <t>Ziehe den Arm rüber, halte den Rücken gerade &amp; Bauch engespannt</t>
   </si>
   <si>
-    <t>07:50 : 08:20</t>
-  </si>
-  <si>
     <t>Halte die Position für ein paar Sekunden</t>
   </si>
   <si>
     <t>Lege deinen linken Arm hinter den Rücken</t>
-  </si>
-  <si>
-    <t>08:20 : 08:26</t>
-  </si>
-  <si>
-    <t>08:26 : 08:43</t>
   </si>
   <si>
     <t>Step 8</t>
@@ -1576,8 +1483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10F13E78-A35E-479F-9F68-61FF6211E1D8}">
   <dimension ref="A1:M132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D124" sqref="D124"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1919,8 +1826,8 @@
       <c r="B38" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C38" t="s">
-        <v>54</v>
+      <c r="C38">
+        <v>4</v>
       </c>
       <c r="D38" s="1"/>
     </row>
@@ -1929,10 +1836,10 @@
         <v>9</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C39" t="s">
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="C39">
+        <v>6</v>
       </c>
       <c r="D39" s="1"/>
     </row>
@@ -1941,10 +1848,10 @@
         <v>11</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C40" t="s">
-        <v>58</v>
+        <v>55</v>
+      </c>
+      <c r="C40">
+        <v>8</v>
       </c>
       <c r="D40" s="1"/>
     </row>
@@ -1953,10 +1860,10 @@
         <v>43</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C41" t="s">
-        <v>60</v>
+        <v>56</v>
+      </c>
+      <c r="C41">
+        <v>13</v>
       </c>
       <c r="D41" s="1"/>
     </row>
@@ -1965,34 +1872,34 @@
         <v>15</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C42" t="s">
-        <v>62</v>
+        <v>57</v>
+      </c>
+      <c r="C42">
+        <v>7</v>
       </c>
       <c r="D42" s="1"/>
     </row>
     <row r="43" spans="1:4" ht="30.75">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C43" t="s">
-        <v>65</v>
+        <v>59</v>
+      </c>
+      <c r="C43">
+        <v>22</v>
       </c>
       <c r="D43" s="1"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C44" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D44" s="1"/>
     </row>
@@ -2006,7 +1913,7 @@
         <v>4</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" s="1" t="s">
@@ -2018,10 +1925,10 @@
         <v>7</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C47" t="s">
-        <v>71</v>
+        <v>64</v>
+      </c>
+      <c r="C47">
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -2029,10 +1936,10 @@
         <v>9</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C48" t="s">
-        <v>73</v>
+        <v>65</v>
+      </c>
+      <c r="C48">
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:4">
@@ -2040,10 +1947,10 @@
         <v>11</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C49" t="s">
-        <v>75</v>
+        <v>66</v>
+      </c>
+      <c r="C49">
+        <v>4</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="30.75">
@@ -2051,7 +1958,7 @@
         <v>43</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
     </row>
     <row r="51" spans="1:4">
@@ -2059,21 +1966,21 @@
         <v>15</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C51" t="s">
-        <v>78</v>
+        <v>68</v>
+      </c>
+      <c r="C51">
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C52" t="s">
-        <v>80</v>
+        <v>69</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:4">
@@ -2086,7 +1993,7 @@
         <v>4</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="1" t="s">
@@ -2100,8 +2007,8 @@
       <c r="B55" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C55" s="4" t="s">
-        <v>82</v>
+      <c r="C55">
+        <v>10</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -2109,10 +2016,10 @@
         <v>9</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>82</v>
+        <v>71</v>
+      </c>
+      <c r="C56">
+        <v>10</v>
       </c>
       <c r="D56" s="1"/>
     </row>
@@ -2121,10 +2028,10 @@
         <v>11</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>82</v>
+        <v>72</v>
+      </c>
+      <c r="C57">
+        <v>10</v>
       </c>
     </row>
     <row r="58" spans="1:4">
@@ -2132,10 +2039,10 @@
         <v>43</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>82</v>
+        <v>73</v>
+      </c>
+      <c r="C58">
+        <v>10</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -2143,21 +2050,21 @@
         <v>15</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>82</v>
+        <v>74</v>
+      </c>
+      <c r="C59">
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>82</v>
+        <v>75</v>
+      </c>
+      <c r="C60">
+        <v>10</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -2170,9 +2077,8 @@
         <v>4</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="C62" s="2"/>
+        <v>76</v>
+      </c>
       <c r="D62" s="1" t="s">
         <v>52</v>
       </c>
@@ -2182,10 +2088,10 @@
         <v>7</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>90</v>
+        <v>77</v>
+      </c>
+      <c r="C63">
+        <v>11</v>
       </c>
       <c r="D63" s="1"/>
     </row>
@@ -2194,10 +2100,10 @@
         <v>9</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>92</v>
+        <v>78</v>
+      </c>
+      <c r="C64">
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:4">
@@ -2205,10 +2111,10 @@
         <v>11</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="C65" s="4" t="s">
-        <v>94</v>
+        <v>79</v>
+      </c>
+      <c r="C65">
+        <v>3</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -2216,10 +2122,10 @@
         <v>43</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>96</v>
+        <v>80</v>
+      </c>
+      <c r="C66">
+        <v>6</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="30.75">
@@ -2227,29 +2133,29 @@
         <v>15</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>98</v>
+        <v>81</v>
+      </c>
+      <c r="C67">
+        <v>40</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="30.75">
       <c r="A68" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="30.75">
       <c r="A69" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B69" s="9" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
     </row>
     <row r="70" spans="1:4">
@@ -2262,7 +2168,7 @@
         <v>4</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>52</v>
@@ -2273,10 +2179,10 @@
         <v>7</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>103</v>
+        <v>85</v>
+      </c>
+      <c r="C72">
+        <v>2</v>
       </c>
     </row>
     <row r="73" spans="1:4">
@@ -2284,13 +2190,13 @@
         <v>9</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C73" s="4" t="s">
-        <v>105</v>
+        <v>86</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
       </c>
       <c r="D73" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
     </row>
     <row r="74" spans="1:4">
@@ -2298,10 +2204,10 @@
         <v>11</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C74" s="4" t="s">
-        <v>108</v>
+        <v>88</v>
+      </c>
+      <c r="C74">
+        <v>7</v>
       </c>
     </row>
     <row r="75" spans="1:4">
@@ -2309,10 +2215,10 @@
         <v>43</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>110</v>
+        <v>89</v>
+      </c>
+      <c r="C75">
+        <v>47</v>
       </c>
     </row>
     <row r="76" spans="1:4">
@@ -2325,11 +2231,11 @@
         <v>4</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="1" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -2337,10 +2243,10 @@
         <v>7</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
     </row>
     <row r="79" spans="1:4">
@@ -2348,7 +2254,7 @@
         <v>29</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
     </row>
     <row r="80" spans="1:4">
@@ -2356,7 +2262,7 @@
         <v>11</v>
       </c>
       <c r="B80" s="5" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
     </row>
     <row r="81" spans="1:13">
@@ -2364,7 +2270,7 @@
         <v>13</v>
       </c>
       <c r="B81" s="5" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
     </row>
     <row r="82" spans="1:13">
@@ -2377,11 +2283,11 @@
         <v>4</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" s="1" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
     </row>
     <row r="84" spans="1:13">
@@ -2389,7 +2295,7 @@
         <v>7</v>
       </c>
       <c r="B84" s="5" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
     </row>
     <row r="85" spans="1:13">
@@ -2397,7 +2303,7 @@
         <v>9</v>
       </c>
       <c r="B85" s="5" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
     </row>
     <row r="86" spans="1:13">
@@ -2405,7 +2311,7 @@
         <v>11</v>
       </c>
       <c r="B86" s="5" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
     </row>
     <row r="87" spans="1:13">
@@ -2413,7 +2319,7 @@
         <v>43</v>
       </c>
       <c r="B87" s="5" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
     </row>
     <row r="88" spans="1:13">
@@ -2421,15 +2327,15 @@
         <v>15</v>
       </c>
       <c r="B88" s="5" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
     </row>
     <row r="89" spans="1:13">
       <c r="A89" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B89" s="5" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
     </row>
     <row r="90" spans="1:13">
@@ -2442,11 +2348,11 @@
         <v>4</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" s="1" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
     </row>
     <row r="92" spans="1:13">
@@ -2454,7 +2360,7 @@
         <v>7</v>
       </c>
       <c r="B92" s="5" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
     </row>
     <row r="93" spans="1:13">
@@ -2462,7 +2368,7 @@
         <v>9</v>
       </c>
       <c r="B93" s="5" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
     </row>
     <row r="94" spans="1:13">
@@ -2470,7 +2376,7 @@
         <v>11</v>
       </c>
       <c r="B94" s="5" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
     </row>
     <row r="95" spans="1:13">
@@ -2483,11 +2389,11 @@
         <v>4</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" s="1" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
@@ -2504,7 +2410,7 @@
         <v>7</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2512,7 +2418,7 @@
         <v>9</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -2520,7 +2426,7 @@
         <v>31</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -2528,7 +2434,7 @@
         <v>13</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -2536,15 +2442,15 @@
         <v>15</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="A102" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
     </row>
     <row r="103" spans="1:4">
@@ -2557,11 +2463,11 @@
         <v>4</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="C104" s="2"/>
       <c r="D104" s="1" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="30.75">
@@ -2569,7 +2475,7 @@
         <v>7</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
     </row>
     <row r="106" spans="1:4">
@@ -2577,7 +2483,7 @@
         <v>9</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="30.75">
@@ -2585,7 +2491,7 @@
         <v>31</v>
       </c>
       <c r="B107" s="5" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
     </row>
     <row r="108" spans="1:4">
@@ -2593,7 +2499,7 @@
         <v>13</v>
       </c>
       <c r="B108" s="5" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="30.75">
@@ -2601,23 +2507,23 @@
         <v>15</v>
       </c>
       <c r="B109" s="5" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="30.75">
       <c r="A110" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B110" s="5" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
     </row>
     <row r="111" spans="1:4">
       <c r="A111" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B111" s="5" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
     </row>
     <row r="112" spans="1:4">
@@ -2630,7 +2536,7 @@
         <v>4</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>146</v>
+        <v>125</v>
       </c>
       <c r="C113" s="2"/>
       <c r="D113" s="1" t="s">
@@ -2644,8 +2550,8 @@
       <c r="B114" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C114" t="s">
-        <v>147</v>
+      <c r="C114">
+        <v>5</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -2653,10 +2559,10 @@
         <v>9</v>
       </c>
       <c r="B115" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="C115" t="s">
-        <v>149</v>
+        <v>126</v>
+      </c>
+      <c r="C115">
+        <v>4</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2664,10 +2570,10 @@
         <v>11</v>
       </c>
       <c r="B116" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="C116" t="s">
-        <v>151</v>
+        <v>127</v>
+      </c>
+      <c r="C116">
+        <v>4</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2675,10 +2581,10 @@
         <v>43</v>
       </c>
       <c r="B117" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="C117" t="s">
-        <v>153</v>
+        <v>128</v>
+      </c>
+      <c r="C117">
+        <v>47</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2686,7 +2592,7 @@
         <v>15</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>154</v>
+        <v>129</v>
       </c>
       <c r="C118" s="7"/>
     </row>
@@ -2700,7 +2606,7 @@
         <v>4</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>155</v>
+        <v>130</v>
       </c>
       <c r="C120" s="2"/>
       <c r="D120" s="1" t="s">
@@ -2712,10 +2618,10 @@
         <v>27</v>
       </c>
       <c r="B121" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="C121" t="s">
-        <v>157</v>
+        <v>131</v>
+      </c>
+      <c r="C121">
+        <v>3</v>
       </c>
     </row>
     <row r="122" spans="1:4">
@@ -2723,10 +2629,10 @@
         <v>9</v>
       </c>
       <c r="B122" s="5" t="s">
-        <v>158</v>
-      </c>
-      <c r="C122" t="s">
-        <v>159</v>
+        <v>132</v>
+      </c>
+      <c r="C122">
+        <v>3</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -2734,10 +2640,10 @@
         <v>11</v>
       </c>
       <c r="B123" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="C123" t="s">
-        <v>161</v>
+        <v>133</v>
+      </c>
+      <c r="C123">
+        <v>3</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="30.75">
@@ -2745,10 +2651,10 @@
         <v>43</v>
       </c>
       <c r="B124" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="C124" t="s">
-        <v>163</v>
+        <v>134</v>
+      </c>
+      <c r="C124">
+        <v>30</v>
       </c>
     </row>
     <row r="125" spans="1:4">
@@ -2756,38 +2662,38 @@
         <v>15</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>164</v>
+        <v>135</v>
       </c>
       <c r="C125" s="7"/>
     </row>
     <row r="126" spans="1:4">
       <c r="A126" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B126" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="C126" t="s">
-        <v>166</v>
+        <v>136</v>
+      </c>
+      <c r="C126">
+        <v>6</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="30.75">
       <c r="A127" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B127" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="C127" t="s">
-        <v>167</v>
+        <v>134</v>
+      </c>
+      <c r="C127">
+        <v>17</v>
       </c>
     </row>
     <row r="128" spans="1:4">
       <c r="A128" t="s">
-        <v>168</v>
+        <v>137</v>
       </c>
       <c r="B128" s="5" t="s">
-        <v>164</v>
+        <v>135</v>
       </c>
     </row>
     <row r="129" spans="1:1">
@@ -2842,7 +2748,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18.75">
       <c r="A1" s="10" t="s">
-        <v>169</v>
+        <v>138</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>3</v>
@@ -2850,274 +2756,274 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>170</v>
+        <v>139</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>172</v>
+        <v>141</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>173</v>
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>174</v>
+        <v>143</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>175</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>176</v>
+        <v>145</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>177</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>178</v>
+        <v>147</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>179</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>180</v>
+        <v>149</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>181</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>182</v>
+        <v>151</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>183</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>184</v>
+        <v>153</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>185</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>186</v>
+        <v>155</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>187</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>188</v>
+        <v>157</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>189</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>190</v>
+        <v>159</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>191</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>192</v>
+        <v>161</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>193</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>194</v>
+        <v>163</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>195</v>
+        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>196</v>
+        <v>165</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>197</v>
+        <v>166</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>198</v>
+        <v>167</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>199</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>200</v>
+        <v>169</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>201</v>
+        <v>170</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>202</v>
+        <v>171</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>203</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>204</v>
+        <v>173</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>205</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>206</v>
+        <v>175</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>207</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>208</v>
+        <v>177</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>209</v>
+        <v>178</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>210</v>
+        <v>179</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>211</v>
+        <v>180</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>212</v>
+        <v>181</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>213</v>
+        <v>182</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>214</v>
+        <v>183</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>215</v>
+        <v>184</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>216</v>
+        <v>185</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>217</v>
+        <v>186</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>218</v>
+        <v>187</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>219</v>
+        <v>188</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>220</v>
+        <v>189</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>221</v>
+        <v>190</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>222</v>
+        <v>191</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>223</v>
+        <v>192</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>224</v>
+        <v>193</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>225</v>
+        <v>194</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>226</v>
+        <v>195</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>227</v>
+        <v>196</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>228</v>
+        <v>197</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>229</v>
+        <v>198</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>230</v>
+        <v>199</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>231</v>
+        <v>200</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>232</v>
+        <v>201</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>233</v>
+        <v>202</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>234</v>
+        <v>203</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>235</v>
+        <v>204</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" s="7" t="s">
-        <v>236</v>
+        <v>205</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>237</v>
+        <v>206</v>
       </c>
     </row>
   </sheetData>
@@ -3179,10 +3085,10 @@
   <sheetData>
     <row r="1" spans="1:2" ht="18.75">
       <c r="A1" s="6" t="s">
-        <v>238</v>
+        <v>207</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>239</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15">
@@ -3191,586 +3097,586 @@
     </row>
     <row r="3" spans="1:2" ht="15">
       <c r="A3" t="s">
-        <v>240</v>
+        <v>209</v>
       </c>
       <c r="B3" t="s">
-        <v>241</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15">
       <c r="A4" t="s">
-        <v>242</v>
+        <v>211</v>
       </c>
       <c r="B4" t="s">
-        <v>243</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15">
       <c r="A5" t="s">
-        <v>244</v>
+        <v>213</v>
       </c>
       <c r="B5" t="s">
-        <v>245</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15">
       <c r="A6" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
       <c r="B6" t="s">
-        <v>247</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30.75">
       <c r="A7" s="5" t="s">
-        <v>248</v>
+        <v>217</v>
       </c>
       <c r="B7" t="s">
-        <v>249</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15">
       <c r="A8" t="s">
-        <v>250</v>
+        <v>219</v>
       </c>
       <c r="B8" t="s">
-        <v>251</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="14.1" customHeight="1">
       <c r="A9" t="s">
-        <v>252</v>
+        <v>221</v>
       </c>
       <c r="B9" t="s">
-        <v>253</v>
+        <v>222</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15">
       <c r="A10" t="s">
-        <v>254</v>
+        <v>223</v>
       </c>
       <c r="B10" t="s">
-        <v>255</v>
+        <v>224</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15">
       <c r="A11" t="s">
-        <v>256</v>
+        <v>225</v>
       </c>
       <c r="B11" t="s">
-        <v>257</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15">
       <c r="A12" t="s">
-        <v>258</v>
+        <v>227</v>
       </c>
       <c r="B12" t="s">
-        <v>259</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15">
       <c r="A13" t="s">
-        <v>260</v>
+        <v>229</v>
       </c>
       <c r="B13" t="s">
-        <v>261</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15">
       <c r="A14" t="s">
-        <v>262</v>
+        <v>231</v>
       </c>
       <c r="B14" t="s">
-        <v>263</v>
+        <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="30.75">
       <c r="A15" s="5" t="s">
-        <v>264</v>
+        <v>233</v>
       </c>
       <c r="B15" t="s">
-        <v>265</v>
+        <v>234</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="30.75">
       <c r="A16" s="5" t="s">
-        <v>266</v>
+        <v>235</v>
       </c>
       <c r="B16" t="s">
-        <v>267</v>
+        <v>236</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15">
       <c r="A17" t="s">
-        <v>268</v>
+        <v>237</v>
       </c>
       <c r="B17" t="s">
-        <v>269</v>
+        <v>238</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15">
       <c r="A18" t="s">
-        <v>270</v>
+        <v>239</v>
       </c>
       <c r="B18" t="s">
-        <v>271</v>
+        <v>240</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15">
       <c r="A19" t="s">
-        <v>272</v>
+        <v>241</v>
       </c>
       <c r="B19" t="s">
-        <v>273</v>
+        <v>242</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15">
       <c r="A20" t="s">
-        <v>274</v>
+        <v>243</v>
       </c>
       <c r="B20" t="s">
-        <v>275</v>
+        <v>244</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="30.75">
       <c r="A21" s="5" t="s">
-        <v>276</v>
+        <v>245</v>
       </c>
       <c r="B21" t="s">
-        <v>277</v>
+        <v>246</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="30.75">
       <c r="A22" s="5" t="s">
-        <v>278</v>
+        <v>247</v>
       </c>
       <c r="B22" t="s">
-        <v>279</v>
+        <v>248</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15">
       <c r="A23" s="5" t="s">
-        <v>280</v>
+        <v>249</v>
       </c>
       <c r="B23" t="s">
-        <v>281</v>
+        <v>250</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15">
       <c r="A24" s="5" t="s">
-        <v>282</v>
+        <v>251</v>
       </c>
       <c r="B24" t="s">
-        <v>283</v>
+        <v>252</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15">
       <c r="A25" s="5" t="s">
-        <v>284</v>
+        <v>253</v>
       </c>
       <c r="B25" t="s">
-        <v>285</v>
+        <v>254</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="30.75">
       <c r="A26" s="5" t="s">
-        <v>286</v>
+        <v>255</v>
       </c>
       <c r="B26" t="s">
-        <v>287</v>
+        <v>256</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15">
       <c r="A27" t="s">
-        <v>288</v>
+        <v>257</v>
       </c>
       <c r="B27" t="s">
-        <v>289</v>
+        <v>258</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15">
       <c r="A28" t="s">
-        <v>290</v>
+        <v>259</v>
       </c>
       <c r="B28" t="s">
-        <v>291</v>
+        <v>260</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15">
       <c r="A29" t="s">
-        <v>292</v>
+        <v>261</v>
       </c>
       <c r="B29" t="s">
-        <v>289</v>
+        <v>258</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15">
       <c r="A30" t="s">
-        <v>293</v>
+        <v>262</v>
       </c>
       <c r="B30" t="s">
-        <v>294</v>
+        <v>263</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15">
       <c r="A31" t="s">
-        <v>295</v>
+        <v>264</v>
       </c>
       <c r="B31" t="s">
-        <v>289</v>
+        <v>258</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15">
       <c r="A32" t="s">
-        <v>296</v>
+        <v>265</v>
       </c>
       <c r="B32" t="s">
-        <v>297</v>
+        <v>266</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15">
       <c r="A33" t="s">
-        <v>298</v>
+        <v>267</v>
       </c>
       <c r="B33" t="s">
-        <v>299</v>
+        <v>268</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15">
       <c r="A34" t="s">
-        <v>300</v>
+        <v>269</v>
       </c>
       <c r="B34" t="s">
-        <v>301</v>
+        <v>270</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15">
       <c r="A35" t="s">
-        <v>302</v>
+        <v>271</v>
       </c>
       <c r="B35" t="s">
-        <v>303</v>
+        <v>272</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15">
       <c r="A36" t="s">
-        <v>304</v>
+        <v>273</v>
       </c>
       <c r="B36" t="s">
-        <v>289</v>
+        <v>258</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>305</v>
+        <v>274</v>
       </c>
       <c r="B37" t="s">
-        <v>289</v>
+        <v>258</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15">
       <c r="A38" t="s">
-        <v>306</v>
+        <v>275</v>
       </c>
       <c r="B38" t="s">
-        <v>289</v>
+        <v>258</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15">
       <c r="A39" t="s">
-        <v>307</v>
+        <v>276</v>
       </c>
       <c r="B39" t="s">
-        <v>289</v>
+        <v>258</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15">
       <c r="A40" t="s">
-        <v>308</v>
+        <v>277</v>
       </c>
       <c r="B40" t="s">
-        <v>289</v>
+        <v>258</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15">
       <c r="A41" t="s">
-        <v>309</v>
+        <v>278</v>
       </c>
       <c r="B41" t="s">
-        <v>289</v>
+        <v>258</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15">
       <c r="A42" t="s">
-        <v>310</v>
+        <v>279</v>
       </c>
       <c r="B42" t="s">
-        <v>289</v>
+        <v>258</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="30.75">
       <c r="A43" s="5" t="s">
-        <v>311</v>
+        <v>280</v>
       </c>
       <c r="B43" t="s">
-        <v>289</v>
+        <v>258</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15">
       <c r="A44" t="s">
-        <v>312</v>
+        <v>281</v>
       </c>
       <c r="B44" t="s">
-        <v>313</v>
+        <v>282</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15">
       <c r="A45" t="s">
-        <v>314</v>
+        <v>283</v>
       </c>
       <c r="B45" t="s">
-        <v>289</v>
+        <v>258</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15">
       <c r="A46" t="s">
-        <v>315</v>
+        <v>284</v>
       </c>
       <c r="B46" t="s">
-        <v>316</v>
+        <v>285</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15">
       <c r="A47" t="s">
-        <v>317</v>
+        <v>286</v>
       </c>
       <c r="B47" t="s">
-        <v>318</v>
+        <v>287</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15">
       <c r="A48" t="s">
-        <v>319</v>
+        <v>288</v>
       </c>
       <c r="B48" t="s">
-        <v>320</v>
+        <v>289</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15">
       <c r="A49" t="s">
-        <v>321</v>
+        <v>290</v>
       </c>
       <c r="B49" t="s">
-        <v>322</v>
+        <v>291</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15">
       <c r="A50" t="s">
-        <v>323</v>
+        <v>292</v>
       </c>
       <c r="B50" t="s">
-        <v>324</v>
+        <v>293</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15">
       <c r="A51" t="s">
-        <v>325</v>
+        <v>294</v>
       </c>
       <c r="B51" t="s">
-        <v>326</v>
+        <v>295</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15">
       <c r="A52" t="s">
-        <v>327</v>
+        <v>296</v>
       </c>
       <c r="B52" t="s">
-        <v>328</v>
+        <v>297</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15">
       <c r="A53" t="s">
-        <v>329</v>
+        <v>298</v>
       </c>
       <c r="B53" t="s">
-        <v>330</v>
+        <v>299</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15">
       <c r="A54" t="s">
-        <v>331</v>
+        <v>300</v>
       </c>
       <c r="B54" t="s">
-        <v>332</v>
+        <v>301</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15">
       <c r="A55" t="s">
-        <v>333</v>
+        <v>302</v>
       </c>
       <c r="B55" t="s">
-        <v>334</v>
+        <v>303</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15">
       <c r="A56" t="s">
-        <v>335</v>
+        <v>304</v>
       </c>
       <c r="B56" t="s">
-        <v>336</v>
+        <v>305</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15">
       <c r="A57" t="s">
-        <v>337</v>
+        <v>306</v>
       </c>
       <c r="B57" t="s">
-        <v>294</v>
+        <v>263</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15">
       <c r="A58" t="s">
-        <v>338</v>
+        <v>307</v>
       </c>
       <c r="B58" t="s">
-        <v>289</v>
+        <v>258</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15">
       <c r="A59" t="s">
-        <v>339</v>
+        <v>308</v>
       </c>
       <c r="B59" t="s">
-        <v>340</v>
+        <v>309</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15">
       <c r="A60" t="s">
-        <v>341</v>
+        <v>310</v>
       </c>
       <c r="B60" t="s">
-        <v>342</v>
+        <v>311</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15">
       <c r="A61" t="s">
-        <v>343</v>
+        <v>312</v>
       </c>
       <c r="B61" t="s">
-        <v>318</v>
+        <v>287</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15">
       <c r="A62" t="s">
-        <v>344</v>
+        <v>313</v>
       </c>
       <c r="B62" t="s">
-        <v>322</v>
+        <v>291</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15">
       <c r="A63" t="s">
-        <v>345</v>
+        <v>314</v>
       </c>
       <c r="B63" t="s">
-        <v>322</v>
+        <v>291</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15">
       <c r="A64" t="s">
-        <v>346</v>
+        <v>315</v>
       </c>
       <c r="B64" t="s">
-        <v>347</v>
+        <v>316</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15">
       <c r="A65" t="s">
-        <v>348</v>
+        <v>317</v>
       </c>
       <c r="B65" t="s">
-        <v>279</v>
+        <v>248</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="30.75">
       <c r="A66" s="5" t="s">
-        <v>349</v>
+        <v>318</v>
       </c>
       <c r="B66" t="s">
-        <v>350</v>
+        <v>319</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="30.75">
       <c r="A67" s="5" t="s">
-        <v>351</v>
+        <v>320</v>
       </c>
       <c r="B67" t="s">
-        <v>352</v>
+        <v>321</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15">
       <c r="A68" s="5" t="s">
-        <v>353</v>
+        <v>322</v>
       </c>
       <c r="B68" t="s">
-        <v>352</v>
+        <v>321</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="15">
       <c r="A69" s="5" t="s">
-        <v>354</v>
+        <v>323</v>
       </c>
       <c r="B69" t="s">
-        <v>352</v>
+        <v>321</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="15">
       <c r="A70" s="5" t="s">
-        <v>355</v>
+        <v>324</v>
       </c>
       <c r="B70" t="s">
-        <v>352</v>
+        <v>321</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="15">
       <c r="A71" s="5" t="s">
-        <v>356</v>
+        <v>325</v>
       </c>
       <c r="B71" t="s">
-        <v>357</v>
+        <v>326</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="30.75">
       <c r="A72" s="5" t="s">
-        <v>358</v>
+        <v>327</v>
       </c>
       <c r="B72" t="s">
-        <v>357</v>
+        <v>326</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="15">
       <c r="A73" s="5" t="s">
-        <v>359</v>
+        <v>328</v>
       </c>
       <c r="B73" t="s">
-        <v>352</v>
+        <v>321</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="15">
       <c r="A74" s="5" t="s">
-        <v>360</v>
+        <v>329</v>
       </c>
       <c r="B74" t="s">
-        <v>352</v>
+        <v>321</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="15">
       <c r="A75" t="s">
-        <v>361</v>
+        <v>330</v>
       </c>
       <c r="B75" t="s">
-        <v>352</v>
+        <v>321</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="15"/>

</xml_diff>

<commit_message>
Some times got updated again
</commit_message>
<xml_diff>
--- a/assets/data/material_database.xlsx
+++ b/assets/data/material_database.xlsx
@@ -2175,7 +2175,7 @@
         <v>244</v>
       </c>
       <c r="C29" s="22">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="3"/>
@@ -3589,7 +3589,7 @@
         <v>316</v>
       </c>
       <c r="C97" s="16">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D97" s="17"/>
       <c r="E97" s="17"/>
@@ -3610,7 +3610,7 @@
         <v>317</v>
       </c>
       <c r="C98" s="16">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D98" s="17"/>
       <c r="E98" s="17"/>
@@ -3652,7 +3652,7 @@
         <v>319</v>
       </c>
       <c r="C100" s="16">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D100" s="17"/>
       <c r="E100" s="17"/>
@@ -3673,7 +3673,7 @@
         <v>317</v>
       </c>
       <c r="C101" s="16">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D101" s="17"/>
       <c r="E101" s="17"/>
@@ -4087,7 +4087,7 @@
         <v>336</v>
       </c>
       <c r="C121" s="23">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D121" s="3"/>
       <c r="E121" s="3"/>
@@ -4108,7 +4108,7 @@
         <v>337</v>
       </c>
       <c r="C122" s="23">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D122" s="3"/>
       <c r="E122" s="3"/>
@@ -4129,7 +4129,7 @@
         <v>338</v>
       </c>
       <c r="C123" s="23">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D123" s="3"/>
       <c r="E123" s="3"/>
@@ -4150,7 +4150,7 @@
         <v>339</v>
       </c>
       <c r="C124" s="23">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D124" s="3"/>
       <c r="E124" s="3"/>
@@ -4192,7 +4192,7 @@
         <v>341</v>
       </c>
       <c r="C126" s="23">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="D126" s="3"/>
       <c r="E126" s="3"/>
@@ -4213,7 +4213,7 @@
         <v>339</v>
       </c>
       <c r="C127" s="23">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D127" s="3"/>
       <c r="E127" s="3"/>

</xml_diff>